<commit_message>
Removed tag in tag
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA_Release\Demo_S012_Vonline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F7F85E-8A47-43DA-993E-C0B269107E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810CA34D-9BC4-4700-A197-2AFEB81307B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="853" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="106">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -3454,10 +3454,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B3:H41"/>
+  <dimension ref="B3:F37"/>
   <sheetViews>
     <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M47" sqref="M47"/>
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3551,12 +3551,12 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>17</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>3</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>3</v>
       </c>
@@ -3595,53 +3595,6 @@
         <v>13</v>
       </c>
       <c r="E37" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="E38" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E39" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F39" s="63" t="s">
-        <v>2</v>
-      </c>
-      <c r="G39" s="64" t="s">
-        <v>18</v>
-      </c>
-      <c r="H39" s="64" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="E40" t="s">
-        <v>3</v>
-      </c>
-      <c r="F40">
-        <v>2222</v>
-      </c>
-      <c r="G40" t="s">
-        <v>13</v>
-      </c>
-      <c r="H40" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="E41" t="s">
-        <v>3</v>
-      </c>
-      <c r="F41">
-        <v>8888</v>
-      </c>
-      <c r="G41" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3656,10 +3609,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B3:W53"/>
+  <dimension ref="B3:Y56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R47" sqref="R47"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3967,7 +3920,7 @@
         <v>0.27111872146118721</v>
       </c>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B33" s="56" t="s">
         <v>61</v>
       </c>
@@ -3998,228 +3951,339 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="P34" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="2:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P35" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q35" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="R35" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="S35" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="T35" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="U35" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="V35" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="W35" s="5"/>
-    </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="R36" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="S36" s="9">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="R37" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="S37" s="9">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="P38" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="R38" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="S38" s="13">
-        <f>G32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="P39" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="R39" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="S39" s="13">
-        <f>H32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="P40" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="R40" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="S40" s="13">
-        <f>I32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="P41" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="R41" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="S41" s="13">
-        <f>J32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34"/>
+      <c r="Y34"/>
+    </row>
+    <row r="35" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+    </row>
+    <row r="36" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+    </row>
+    <row r="37" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+    </row>
+    <row r="38" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="S38" s="13"/>
+    </row>
+    <row r="39" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="S39" s="13"/>
+    </row>
+    <row r="40" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="S40" s="13"/>
+    </row>
+    <row r="41" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+      <c r="S41" s="13"/>
+    </row>
+    <row r="42" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42"/>
       <c r="P42"/>
       <c r="Q42"/>
-      <c r="R42" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="T42" s="13">
-        <v>0.9</v>
-      </c>
-      <c r="U42" s="13">
-        <v>0.95</v>
-      </c>
-      <c r="V42" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="E45" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="46" spans="2:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E46" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H46" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K46" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L46" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="G47" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H47" s="9">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="G48" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H48" s="9">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="49" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E49" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H49" s="13" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="50" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E50" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G50" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H50" s="13" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="51" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E51" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G51" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H51" s="13" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="52" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E52" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G52" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H52" s="13" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="53" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="T42" s="13"/>
+      <c r="U42" s="13"/>
+    </row>
+    <row r="43" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+      <c r="O43"/>
+      <c r="P43"/>
+      <c r="Q43"/>
+    </row>
+    <row r="44" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44"/>
+      <c r="P44"/>
+      <c r="Q44"/>
+    </row>
+    <row r="45" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+      <c r="Q45"/>
+    </row>
+    <row r="46" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+      <c r="O46"/>
+      <c r="P46"/>
+      <c r="Q46"/>
+    </row>
+    <row r="47" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
+      <c r="O47"/>
+      <c r="P47"/>
+      <c r="Q47"/>
+    </row>
+    <row r="48" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
+      <c r="O48"/>
+      <c r="P48"/>
+      <c r="Q48"/>
+    </row>
+    <row r="49" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49"/>
+      <c r="K49"/>
+      <c r="L49"/>
+      <c r="M49"/>
+      <c r="N49"/>
+      <c r="O49"/>
+      <c r="P49"/>
+      <c r="Q49"/>
+    </row>
+    <row r="50" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+      <c r="O50"/>
+      <c r="P50"/>
+      <c r="Q50"/>
+    </row>
+    <row r="51" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+      <c r="J51"/>
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51"/>
+      <c r="O51"/>
+      <c r="P51"/>
+      <c r="Q51"/>
+    </row>
+    <row r="52" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D52"/>
+      <c r="E52"/>
+      <c r="F52"/>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+      <c r="N52"/>
+      <c r="O52"/>
+      <c r="P52"/>
+      <c r="Q52"/>
+    </row>
+    <row r="53" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D53"/>
       <c r="E53"/>
       <c r="F53"/>
-      <c r="G53" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I53" s="13">
-        <v>0.9</v>
-      </c>
-      <c r="J53" s="13">
-        <v>0.95</v>
-      </c>
-      <c r="K53" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L53" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="I53"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53"/>
+      <c r="N53"/>
+      <c r="O53"/>
+      <c r="P53"/>
+      <c r="Q53"/>
+    </row>
+    <row r="54" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D54"/>
+      <c r="E54"/>
+      <c r="F54"/>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+      <c r="N54"/>
+      <c r="O54"/>
+      <c r="P54"/>
+      <c r="Q54"/>
+    </row>
+    <row r="55" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
+      <c r="H55"/>
+      <c r="I55"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55"/>
+      <c r="M55"/>
+      <c r="N55"/>
+      <c r="O55"/>
+      <c r="P55"/>
+      <c r="Q55"/>
+    </row>
+    <row r="56" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D56"/>
+      <c r="E56"/>
+      <c r="F56"/>
+      <c r="G56"/>
+      <c r="H56"/>
+      <c r="I56"/>
+      <c r="J56"/>
+      <c r="K56"/>
+      <c r="L56"/>
+      <c r="M56"/>
+      <c r="N56"/>
+      <c r="O56"/>
+      <c r="P56"/>
+      <c r="Q56"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -4232,10 +4296,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B2:U31"/>
+  <dimension ref="B2:S29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27:U31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4413,7 +4477,7 @@
         <v>1.05555</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>91</v>
       </c>
@@ -4424,7 +4488,7 @@
         <v>4.1868000000000002E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>92</v>
       </c>
@@ -4435,7 +4499,7 @@
         <v>41.868000000000002</v>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>93</v>
       </c>
@@ -4446,7 +4510,7 @@
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>94</v>
       </c>
@@ -4457,7 +4521,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>100</v>
       </c>
@@ -4468,7 +4532,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>102</v>
       </c>
@@ -4482,7 +4546,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="2:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>104</v>
       </c>
@@ -4511,7 +4575,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>95</v>
       </c>
@@ -4540,7 +4604,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>96</v>
       </c>
@@ -4569,7 +4633,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>97</v>
       </c>
@@ -4598,7 +4662,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>98</v>
       </c>
@@ -4608,11 +4672,8 @@
       <c r="D27" s="65">
         <v>2.7777769999999999</v>
       </c>
-      <c r="P27" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="2:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>99</v>
       </c>
@@ -4622,26 +4683,8 @@
       <c r="D28" s="65">
         <v>3.6</v>
       </c>
-      <c r="P28" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q28" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="R28" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="S28" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="T28" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="U28" s="14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>38</v>
       </c>
@@ -4650,64 +4693,6 @@
       </c>
       <c r="D29" s="65">
         <v>1</v>
-      </c>
-      <c r="P29" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q29" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="R29" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="S29" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="T29" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="U29" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="P30" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q30" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="R30" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="S30" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="T30" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="U30" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="P31" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>38</v>
-      </c>
-      <c r="R31" t="s">
-        <v>38</v>
-      </c>
-      <c r="S31" t="s">
-        <v>38</v>
-      </c>
-      <c r="T31" t="s">
-        <v>38</v>
-      </c>
-      <c r="U31" s="12" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>